<commit_message>
Boat and Chair conformations; molecule d always adopt chair after little minimisation
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -386,8 +386,8 @@
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -803,51 +803,123 @@
       <c r="A17" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="B17" s="0" t="n">
+        <v>-5.09</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>-1.75</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>-12.31</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>-6.12</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>-9.74</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1.42</v>
+      </c>
       <c r="K17" s="0" t="n">
         <f aca="false">(F17+G17)-(B17+C17)-H17</f>
-        <v>0</v>
+        <v>-10.07</v>
       </c>
       <c r="L17" s="0" t="n">
         <f aca="false">(F17+G17)-(D17+E17)-I17</f>
-        <v>0</v>
+        <v>-5.68</v>
       </c>
       <c r="N17" s="12" t="n">
         <f aca="false">(-1/(2.303*0.592))*(K17-L17)</f>
-        <v>-0</v>
+        <v>3.21994812876272</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="B18" s="0" t="n">
+        <v>-2.8</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>-3.36</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>4.58</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>-13.93</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>-4.4</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>-11.87</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>2.47</v>
+      </c>
       <c r="K18" s="0" t="n">
         <f aca="false">(F18+G18)-(B18+C18)-H18</f>
-        <v>0</v>
+        <v>-11.86</v>
       </c>
       <c r="L18" s="0" t="n">
         <f aca="false">(F18+G18)-(D18+E18)-I18</f>
-        <v>0</v>
+        <v>-9.39</v>
       </c>
       <c r="N18" s="12" t="n">
         <f aca="false">(-1/(2.303*0.592))*(K18-L18)</f>
-        <v>-0</v>
+        <v>1.81167924329018</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="B19" s="0" t="n">
+        <v>-1.49</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>-3.82</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>6.76</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>-13.93</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>-3.14</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>-12.35</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>2.57</v>
+      </c>
       <c r="K19" s="0" t="n">
         <f aca="false">(F19+G19)-(B19+C19)-H19</f>
-        <v>0</v>
+        <v>-12.05</v>
       </c>
       <c r="L19" s="0" t="n">
         <f aca="false">(F19+G19)-(D19+E19)-I19</f>
-        <v>0</v>
+        <v>-10.89</v>
       </c>
       <c r="N19" s="12" t="n">
         <f aca="false">(-1/(2.303*0.592))*(K19-L19)</f>
-        <v>-0</v>
+        <v>0.850829118306322</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -918,27 +990,63 @@
       <c r="A25" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="B25" s="12" t="n">
+        <f aca="false">AVERAGE(N9,N17)</f>
+        <v>3.09892502141742</v>
+      </c>
+      <c r="C25" s="12" t="n">
+        <f aca="false">STDEV(N9,N17)/SQRT(2)</f>
+        <v>0.121023107345295</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="G25" s="12" t="n">
+        <f aca="false">ABS(((N9-E25)+(N17-E25))/2)</f>
+        <v>0.321074978582575</v>
+      </c>
       <c r="N25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="B26" s="12" t="n">
+        <f aca="false">AVERAGE(N10,N18)</f>
+        <v>1.69432350283414</v>
+      </c>
+      <c r="C26" s="12" t="n">
+        <f aca="false">STDEV(N10,N18)/SQRT(2)</f>
+        <v>0.117355740456047</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="G26" s="12" t="n">
+        <f aca="false">ABS(((N10-E26)+(N18-E26))/2)</f>
+        <v>1.04567649716586</v>
+      </c>
       <c r="N26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="B27" s="12" t="n">
+        <f aca="false">AVERAGE(N11,N19)</f>
+        <v>0.931511189869851</v>
+      </c>
+      <c r="C27" s="12" t="n">
+        <f aca="false">STDEV(N11,N19)/SQRT(2)</f>
+        <v>0.080682071563529</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="G27" s="12" t="n">
+        <f aca="false">ABS(((N11-E27)+(N19-E27))/2)</f>
+        <v>1.74848881013015</v>
+      </c>
       <c r="N27" s="12"/>
     </row>
   </sheetData>

</xml_diff>